<commit_message>
Rafael out 2017 todo: rafael_ano rafael_maj..
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RUM 17.xlsx
+++ b/formats/excel/Formats RUM 17.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81">
   <si>
     <t>position</t>
   </si>
@@ -247,25 +247,7 @@
     <t>Numéro d'innovation</t>
   </si>
   <si>
-    <t>NBIVGANT</t>
-  </si>
-  <si>
-    <t>Nombre d’IVG antérieures</t>
-  </si>
-  <si>
-    <t>ANIVGPREC</t>
-  </si>
-  <si>
-    <t>Année de l’IVG précédente</t>
-  </si>
-  <si>
     <t>Fil2</t>
-  </si>
-  <si>
-    <t>NBNAIVIVANT</t>
-  </si>
-  <si>
-    <t>Nombres de naissances vivantes antérieures</t>
   </si>
   <si>
     <t>ZONRES</t>
@@ -283,9 +265,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -318,22 +300,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -347,9 +339,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -371,11 +369,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -387,16 +384,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -411,14 +422,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -431,28 +435,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -469,25 +451,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,19 +517,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,6 +577,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -530,120 +626,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,15 +663,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -701,6 +674,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,6 +719,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -730,166 +736,142 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1220,10 +1202,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:F42"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1984,124 +1966,58 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="1">
+    <row r="37" spans="1:5">
+      <c r="A37">
         <v>178</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="1">
-        <v>2</v>
+      <c r="C37">
+        <v>12</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="1" t="s">
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>190</v>
+      </c>
+      <c r="B38" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="1">
-        <v>180</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <f>C38+A38-A39</f>
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="1">
-        <v>4</v>
-      </c>
-      <c r="D38" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="1" t="s">
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>193</v>
+      </c>
+      <c r="B39" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="1">
-        <v>184</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="1">
-        <v>4</v>
-      </c>
-      <c r="D39" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="1">
-        <v>188</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="1">
-        <v>2</v>
-      </c>
-      <c r="D40" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="1">
-        <v>190</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="1">
-        <v>3</v>
-      </c>
-      <c r="D41" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" s="1">
-        <v>193</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="1"/>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>